<commit_message>
Peter's code testdata updated
</commit_message>
<xml_diff>
--- a/SeleniumCSharpMSTest/DataManager/TestData.xlsx
+++ b/SeleniumCSharpMSTest/DataManager/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeleniumCSharpMSTest\SeleniumCSharpMSTest\DataManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THI1804359\source\repos\IthmaarCRM\SeleniumCSharpMSTest\DataManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870E4E33-BE83-468B-852D-D872A7CF5AE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A324EF7-55CB-4034-B910-890DD39BD4FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="24" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="25" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerCreation" sheetId="1" r:id="rId1"/>
@@ -41,6 +41,9 @@
     <sheet name="Collection_LatePayment" sheetId="27" r:id="rId26"/>
     <sheet name="CorporateCustomer" sheetId="3" r:id="rId27"/>
     <sheet name="RejectionReasons" sheetId="28" r:id="rId28"/>
+    <sheet name="SalesProspect" sheetId="29" r:id="rId29"/>
+    <sheet name="Reports" sheetId="30" r:id="rId30"/>
+    <sheet name="Servicerequest" sheetId="31" r:id="rId31"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="214">
   <si>
     <t>Password</t>
   </si>
@@ -534,13 +537,181 @@
   </si>
   <si>
     <t>500300001690005</t>
+  </si>
+  <si>
+    <t>Mobilenumber</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Monthlyliabilities</t>
+  </si>
+  <si>
+    <t>Retailcustomer</t>
+  </si>
+  <si>
+    <t>IDnumber</t>
+  </si>
+  <si>
+    <t>IDtype</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Monthlysalary</t>
+  </si>
+  <si>
+    <t>Dateofbirth</t>
+  </si>
+  <si>
+    <t>Lenghtofservice</t>
+  </si>
+  <si>
+    <t>Employer</t>
+  </si>
+  <si>
+    <t>Corpproduct</t>
+  </si>
+  <si>
+    <t>Netprofit</t>
+  </si>
+  <si>
+    <t>Equity</t>
+  </si>
+  <si>
+    <t>Turnover</t>
+  </si>
+  <si>
+    <t>8089493647</t>
+  </si>
+  <si>
+    <t>Testingauto1</t>
+  </si>
+  <si>
+    <t>newauto</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>ABCD1474445</t>
+  </si>
+  <si>
+    <t>PASSPORT</t>
+  </si>
+  <si>
+    <t>Mastercard Corporate</t>
+  </si>
+  <si>
+    <t>18/02/1993</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Searchrecords</t>
+  </si>
+  <si>
+    <t>Numberofdays</t>
+  </si>
+  <si>
+    <t>agingSearchrecords</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>AverageCaseClosuresearch</t>
+  </si>
+  <si>
+    <t>Neglected Cases</t>
+  </si>
+  <si>
+    <t>aging Report</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>Discription</t>
+  </si>
+  <si>
+    <t>Corparatecustomer</t>
+  </si>
+  <si>
+    <t>Documentname</t>
+  </si>
+  <si>
+    <t>Posttext</t>
+  </si>
+  <si>
+    <t>Cancelreason</t>
+  </si>
+  <si>
+    <t>Canceldiscription</t>
+  </si>
+  <si>
+    <t>Categorychangereason</t>
+  </si>
+  <si>
+    <t>Phonecallsubject</t>
+  </si>
+  <si>
+    <t>Appoinmentsubject</t>
+  </si>
+  <si>
+    <t>Al Malkiya Wll</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Documentmissing</t>
+  </si>
+  <si>
+    <t>Collection Documents</t>
+  </si>
+  <si>
+    <t>Information Invalid</t>
+  </si>
+  <si>
+    <t>Information missing</t>
+  </si>
+  <si>
+    <t>Categorychangetesting</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Meeting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,8 +725,15 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,6 +743,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,10 +788,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -628,8 +816,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink 2" xfId="1" xr:uid="{C93228DE-93D5-4CFE-9A92-B7E9A61548C6}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2355,7 +2550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0E3C73-C98C-4A15-AE18-4A48F8B1F078}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -2383,6 +2578,465 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15ECDCB8-13BF-4C7F-AD89-825C7D126401}">
+  <dimension ref="A1:BJ2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="143.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="53.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="79.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="95" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="25.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="20.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="22.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="20.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="19.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="18" style="3" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="41.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="63" max="16384" width="9.109375" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:62" s="14" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD1" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AP1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="AR1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS1" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT1" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="AU1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="AV1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="AZ1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BA1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="BB1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="BC1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="BD1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="BE1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="BF1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="BG1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="BI1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="BJ1" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BH2" s="2">
+        <v>18500</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{516D8584-EC5B-4172-BF1C-AAB7C7511969}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2425,6 +3079,200 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6F8263-7E51-46F3-8DBD-E4D06EB5005D}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{46C1CDDA-6E99-4FF7-B903-FA9365714677}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280FB8DC-7582-4A39-ACC8-1B53CBCA8AA9}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I1" t="s">
+        <v>199</v>
+      </c>
+      <c r="J1" t="s">
+        <v>200</v>
+      </c>
+      <c r="K1" t="s">
+        <v>201</v>
+      </c>
+      <c r="L1" t="s">
+        <v>202</v>
+      </c>
+      <c r="M1" t="s">
+        <v>203</v>
+      </c>
+      <c r="N1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I2" t="s">
+        <v>206</v>
+      </c>
+      <c r="J2" t="s">
+        <v>209</v>
+      </c>
+      <c r="K2" t="s">
+        <v>210</v>
+      </c>
+      <c r="L2" t="s">
+        <v>211</v>
+      </c>
+      <c r="M2" t="s">
+        <v>212</v>
+      </c>
+      <c r="N2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DB02159F-7F11-4630-B2A0-3B5113B8743D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Commiting test data excel
</commit_message>
<xml_diff>
--- a/SeleniumCSharpMSTest/DataManager/TestData.xlsx
+++ b/SeleniumCSharpMSTest/DataManager/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THI1804359\source\repos\IthmaarCRM\SeleniumCSharpMSTest\DataManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\THI1709284\source\repos\IthmaarCRM\SeleniumCSharpMSTest\DataManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A324EF7-55CB-4034-B910-890DD39BD4FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3ED5A0-A2B9-4BBB-96C3-117D9ED31592}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="25" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="21" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerCreation" sheetId="1" r:id="rId1"/>
@@ -2244,9 +2244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC700229-3B71-447B-81CA-4CE66CECFD55}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2585,13 +2583,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15ECDCB8-13BF-4C7F-AD89-825C7D126401}">
   <dimension ref="A1:BJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.109375" style="3" bestFit="1" customWidth="1"/>

</xml_diff>